<commit_message>
Anaysis of Polybius fragments.
</commit_message>
<xml_diff>
--- a/R_files/Rresults/statsRelPos/stats_Oct11/PolybiusAnalysis.xlsx
+++ b/R_files/Rresults/statsRelPos/stats_Oct11/PolybiusAnalysis.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2219" uniqueCount="565">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2223" uniqueCount="565">
   <si>
     <t>Aeschylus</t>
   </si>
@@ -2547,7 +2547,7 @@
       <pane xSplit="1" ySplit="3" topLeftCell="J4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="N1" sqref="N1:O21"/>
+      <selection pane="bottomRight" activeCell="P1" sqref="P1:Q18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -62022,13 +62022,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:O21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="I15" sqref="I15"/>
+      <selection pane="bottomRight" activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -62036,7 +62036,7 @@
     <col min="1" max="1" width="23.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>557</v>
       </c>
@@ -62052,8 +62052,14 @@
       <c r="F1">
         <v>7</v>
       </c>
+      <c r="K1">
+        <v>8</v>
+      </c>
+      <c r="L1">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>558</v>
       </c>
@@ -62072,8 +62078,14 @@
       <c r="H2" t="s">
         <v>564</v>
       </c>
+      <c r="K2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L2" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>559</v>
       </c>
@@ -62095,8 +62107,14 @@
       <c r="I3" t="s">
         <v>561</v>
       </c>
+      <c r="K3" t="s">
+        <v>560</v>
+      </c>
+      <c r="L3" t="s">
+        <v>561</v>
+      </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -62120,8 +62138,22 @@
         <f>STANDARDIZE(H4,$H$20,$H$21)</f>
         <v>-1.0003485063915851</v>
       </c>
+      <c r="K4">
+        <v>1.34972704963189E-2</v>
+      </c>
+      <c r="L4">
+        <v>0.44354138017401201</v>
+      </c>
+      <c r="N4">
+        <f>K4/B4</f>
+        <v>0.22906927326816778</v>
+      </c>
+      <c r="O4">
+        <f>STANDARDIZE(N4,$N$20,$N$21)</f>
+        <v>-0.76743654399838557</v>
+      </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -62145,8 +62177,22 @@
         <f t="shared" ref="I5:I18" si="1">STANDARDIZE(H5,$H$20,$H$21)</f>
         <v>-0.52947071916499866</v>
       </c>
+      <c r="K5">
+        <v>1.9436391047199301E-2</v>
+      </c>
+      <c r="L5">
+        <v>1.76494026777483</v>
+      </c>
+      <c r="N5">
+        <f t="shared" ref="N5:N18" si="2">K5/B5</f>
+        <v>0.44836811128945825</v>
+      </c>
+      <c r="O5">
+        <f t="shared" ref="O5:O18" si="3">STANDARDIZE(N5,$N$20,$N$21)</f>
+        <v>1.4546828575316573</v>
+      </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -62170,8 +62216,22 @@
         <f t="shared" si="1"/>
         <v>1.7387944506513289</v>
       </c>
+      <c r="K6">
+        <v>1.0238203360442601E-2</v>
+      </c>
+      <c r="L6">
+        <v>-0.281570637854485</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="2"/>
+        <v>0.40722495894909838</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="3"/>
+        <v>1.0377859971536558</v>
+      </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -62195,8 +62255,22 @@
         <f t="shared" si="1"/>
         <v>0.47044077817539054</v>
       </c>
+      <c r="K7">
+        <v>1.34796841902561E-2</v>
+      </c>
+      <c r="L7">
+        <v>0.439628591223304</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="2"/>
+        <v>0.40816326530612174</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="3"/>
+        <v>1.047293702617732</v>
+      </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -62220,8 +62294,22 @@
         <f t="shared" si="1"/>
         <v>0.19811381905367409</v>
       </c>
+      <c r="K8">
+        <v>1.8353576248313099E-2</v>
+      </c>
+      <c r="L8">
+        <v>1.52402408187355</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="2"/>
+        <v>0.37988826815642457</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="3"/>
+        <v>0.76078776254317093</v>
+      </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -62245,8 +62333,22 @@
         <f t="shared" si="1"/>
         <v>6.1492307400922153E-2</v>
       </c>
+      <c r="K9">
+        <v>1.41734312588584E-2</v>
+      </c>
+      <c r="L9">
+        <v>0.593980838643419</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="2"/>
+        <v>0.35483870967741921</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="3"/>
+        <v>0.50696466708949051</v>
+      </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -62270,8 +62372,22 @@
         <f t="shared" si="1"/>
         <v>-0.38723271302855189</v>
       </c>
+      <c r="K10">
+        <v>1.3375413285241999E-2</v>
+      </c>
+      <c r="L10">
+        <v>0.416429288108568</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="2"/>
+        <v>0.29865771812080655</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="3"/>
+        <v>-6.2308168378175828E-2</v>
+      </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -62295,8 +62411,22 @@
         <f t="shared" si="1"/>
         <v>-0.4489938897584666</v>
       </c>
+      <c r="K11">
+        <v>1.4936109337493E-2</v>
+      </c>
+      <c r="L11">
+        <v>0.76366959240275101</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="2"/>
+        <v>0.35517970401691284</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="3"/>
+        <v>0.51041990718304353</v>
+      </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -62320,8 +62450,22 @@
         <f t="shared" si="1"/>
         <v>-0.69747692982392651</v>
       </c>
+      <c r="K12">
+        <v>3.2018874283788299E-3</v>
+      </c>
+      <c r="L12">
+        <v>-1.8470852566912099</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="2"/>
+        <v>9.2682926829268306E-2</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="3"/>
+        <v>-2.149417174904662</v>
+      </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -62345,8 +62489,22 @@
         <f t="shared" si="1"/>
         <v>-0.84681706697342862</v>
       </c>
+      <c r="K13">
+        <v>1.25217603762636E-2</v>
+      </c>
+      <c r="L13">
+        <v>0.226499483744865</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="2"/>
+        <v>0.28778661675245604</v>
+      </c>
+      <c r="O13">
+        <f t="shared" si="3"/>
+        <v>-0.17246326762346326</v>
+      </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -62370,8 +62528,22 @@
         <f t="shared" si="1"/>
         <v>0.27880454186644871</v>
       </c>
+      <c r="K14">
+        <v>8.9649156813335906E-3</v>
+      </c>
+      <c r="L14">
+        <v>-0.56486526175650298</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="2"/>
+        <v>0.31569965870307148</v>
+      </c>
+      <c r="O14">
+        <f t="shared" si="3"/>
+        <v>0.11037503938189722</v>
+      </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>11</v>
       </c>
@@ -62395,8 +62567,22 @@
         <f t="shared" si="1"/>
         <v>2.4038709170261412</v>
       </c>
+      <c r="K15" s="2">
+        <v>8.5892764185320093E-3</v>
+      </c>
+      <c r="L15" s="2">
+        <v>-0.64844149156238096</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="2"/>
+        <v>0.32398316970547014</v>
+      </c>
+      <c r="O15">
+        <f t="shared" si="3"/>
+        <v>0.19431050697170088</v>
+      </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>12</v>
       </c>
@@ -62420,8 +62606,22 @@
         <f t="shared" si="1"/>
         <v>0.43281357018682404</v>
       </c>
+      <c r="K16" s="2">
+        <v>6.0893797089482896E-3</v>
+      </c>
+      <c r="L16" s="2">
+        <v>-1.2046451757376699</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="2"/>
+        <v>0.22736030828516407</v>
+      </c>
+      <c r="O16">
+        <f t="shared" si="3"/>
+        <v>-0.78475320777796898</v>
+      </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -62445,8 +62645,22 @@
         <f t="shared" si="1"/>
         <v>-1.30138602354842</v>
       </c>
+      <c r="K17">
+        <v>8.1297334303196307E-3</v>
+      </c>
+      <c r="L17">
+        <v>-0.75068551712582698</v>
+      </c>
+      <c r="N17">
+        <f t="shared" si="2"/>
+        <v>0.14253563390847709</v>
+      </c>
+      <c r="O17">
+        <f t="shared" si="3"/>
+        <v>-1.644267815158629</v>
+      </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -62470,39 +62684,69 @@
         <f t="shared" si="1"/>
         <v>-0.37260453567134544</v>
       </c>
+      <c r="K18">
+        <v>7.5691046710994001E-3</v>
+      </c>
+      <c r="L18">
+        <v>-0.87542018321722603</v>
+      </c>
+      <c r="N18">
+        <f t="shared" si="2"/>
+        <v>0.3006644518272425</v>
+      </c>
+      <c r="O18">
+        <f t="shared" si="3"/>
+        <v>-4.1974262631066059E-2</v>
+      </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>562</v>
       </c>
       <c r="B20">
-        <f t="shared" ref="B20:C20" si="2">AVERAGE(B4:B18)</f>
+        <f t="shared" ref="B20" si="4">AVERAGE(B4:B18)</f>
         <v>3.8499435383924932E-2</v>
       </c>
       <c r="E20">
-        <f t="shared" ref="E20:F20" si="3">AVERAGE(E4:E18)</f>
+        <f t="shared" ref="E20" si="5">AVERAGE(E4:E18)</f>
         <v>1.3223795921367432E-2</v>
       </c>
       <c r="H20">
         <f>AVERAGE(H4:H18)</f>
         <v>0.36660143252458899</v>
       </c>
+      <c r="K20">
+        <f>AVERAGE(K4:K18)</f>
+        <v>1.1503742462599918E-2</v>
+      </c>
+      <c r="N20">
+        <f t="shared" ref="L20:N20" si="6">AVERAGE(N4:N18)</f>
+        <v>0.30480685165303728</v>
+      </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>563</v>
       </c>
       <c r="B21">
-        <f t="shared" ref="B21:C21" si="4">_xlfn.STDEV.S(B4:B18)</f>
+        <f t="shared" ref="B21" si="7">_xlfn.STDEV.S(B4:B18)</f>
         <v>1.1162742861389286E-2</v>
       </c>
       <c r="E21">
-        <f t="shared" ref="E21:F21" si="5">_xlfn.STDEV.S(E4:E18)</f>
+        <f t="shared" ref="E21" si="8">_xlfn.STDEV.S(E4:E18)</f>
         <v>2.8146104665171092E-3</v>
       </c>
       <c r="H21">
         <f>_xlfn.STDEV.S(H4:H18)</f>
         <v>0.12346448171164433</v>
+      </c>
+      <c r="K21">
+        <f>_xlfn.STDEV.S(K4:K18)</f>
+        <v>4.4945705695754665E-3</v>
+      </c>
+      <c r="N21">
+        <f t="shared" ref="L21:N21" si="9">_xlfn.STDEV.S(N4:N18)</f>
+        <v>9.8689043383668767E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>